<commit_message>
Update cascade to use characteristics for which data is provided
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_hiv.xlsx
+++ b/tests/frameworks/framework_hiv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/frameworks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C98B16C1-D993-1343-BE95-B9B0A5502A78}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3176607-C8C8-4B03-A7A5-6A059A6FE31D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="14180" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Parameters" sheetId="6" r:id="rId5"/>
     <sheet name="Cascades" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -1024,7 +1024,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="76">
   <si>
     <t>Code Name</t>
   </si>
@@ -1252,21 +1252,6 @@
   </si>
   <si>
     <t>Virally suppressed (comp)</t>
-  </si>
-  <si>
-    <t>undx,dx,linked,tx,lost,vs</t>
-  </si>
-  <si>
-    <t>dx,linked,tx,lost,vs</t>
-  </si>
-  <si>
-    <t>linked,tx,lost,vs</t>
-  </si>
-  <si>
-    <t>linked,tx,vs</t>
-  </si>
-  <si>
-    <t>tx,vs</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1259,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _k_r_._-;\-* #,##0.00\ _k_r_._-;_-* &quot;-&quot;??\ _k_r_._-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1331,7 +1316,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1348,7 +1333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1699,13 +1684,13 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1713,7 +1698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
@@ -1721,7 +1706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1729,35 +1714,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
     </row>
@@ -1775,18 +1760,18 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1812,7 +1797,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -1836,7 +1821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>20</v>
       </c>
@@ -1860,7 +1845,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1884,7 +1869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -1908,7 +1893,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -1932,7 +1917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -1978,9 +1963,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="str">
         <f>Compartments!$A$2</f>
         <v>undx</v>
@@ -2006,7 +1991,7 @@
         <v>vs</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>Compartments!$A$2</f>
         <v>undx</v>
@@ -2015,7 +2000,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f>Compartments!$A$3</f>
         <v>dx</v>
@@ -2024,7 +2009,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f>Compartments!$A$4</f>
         <v>linked</v>
@@ -2036,7 +2021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f>Compartments!$A$5</f>
         <v>tx</v>
@@ -2048,7 +2033,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f>Compartments!$A$6</f>
         <v>lost</v>
@@ -2057,7 +2042,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f>Compartments!$A$7</f>
         <v>vs</v>
@@ -2079,20 +2064,20 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2115,7 +2100,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -2138,7 +2123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -2161,7 +2146,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>60</v>
       </c>
@@ -2184,7 +2169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>62</v>
       </c>
@@ -2207,7 +2192,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -2230,7 +2215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>68</v>
       </c>
@@ -2253,7 +2238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2261,19 +2246,19 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
     </row>
   </sheetData>
@@ -2295,21 +2280,21 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2344,7 +2329,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -2371,7 +2356,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -2400,7 +2385,7 @@
       </c>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>69</v>
       </c>
@@ -2425,7 +2410,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>41</v>
       </c>
@@ -2452,7 +2437,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -2481,7 +2466,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -2510,7 +2495,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>55</v>
       </c>
@@ -2539,7 +2524,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
@@ -2570,7 +2555,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2581,7 +2566,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2592,7 +2577,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2603,7 +2588,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2614,7 +2599,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2625,7 +2610,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2636,7 +2621,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2647,19 +2632,19 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -2685,16 +2670,16 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -2702,74 +2687,74 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>

</xml_diff>

<commit_message>
Improve calibration workflow based on can calibrate column
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_hiv.xlsx
+++ b/tests/frameworks/framework_hiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3176607-C8C8-4B03-A7A5-6A059A6FE31D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D65937-A9F0-4EAC-AE87-FE8AFC123CB8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Pages" sheetId="8" r:id="rId1"/>
@@ -1757,7 +1757,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,7 +1814,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
@@ -1838,7 +1838,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
@@ -1862,7 +1862,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
@@ -1886,7 +1886,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
@@ -1910,7 +1910,7 @@
         <v>7</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
@@ -1934,7 +1934,7 @@
         <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
@@ -2063,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2669,7 +2669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5680499-D84A-1B4F-B644-03899BDE28FE}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+    <sheetView zoomScale="179" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update progbooks with new calibration defaults and targeting heading name
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_hiv.xlsx
+++ b/tests/frameworks/framework_hiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2567B380-EC90-446C-B075-E45998F37313}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BAA615-B9F4-48D3-974E-999C155647A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -409,30 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This column marks whether compartment size data can be rescaled
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>during model calibration processes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{1463AD83-63D4-EC46-A82A-37905E1D406B}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{1463AD83-63D4-EC46-A82A-37905E1D406B}">
       <text>
         <r>
           <rPr>
@@ -619,21 +596,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column marks whether characteristic size data can be rescaled
-during model calibration processes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{A922DFF6-C9D0-AC4E-B73F-8ED95E92610A}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{A922DFF6-C9D0-AC4E-B73F-8ED95E92610A}">
       <text>
         <r>
           <rPr>
@@ -933,21 +896,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column marks whether parameter data can be rescaled
-during model calibration processes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{A6070E97-93A6-7543-9DAB-DE6A5FB7C74E}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{A6070E97-93A6-7543-9DAB-DE6A5FB7C74E}">
       <text>
         <r>
           <rPr>
@@ -1025,7 +974,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t>Code Name</t>
   </si>
@@ -1045,9 +994,6 @@
     <t>Setup Weight</t>
   </si>
   <si>
-    <t>Can Calibrate</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
@@ -1072,9 +1018,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>Is Impact</t>
-  </si>
-  <si>
     <t>Undiagnosed</t>
   </si>
   <si>
@@ -1262,6 +1205,9 @@
   </si>
   <si>
     <t>An HIV cascade</t>
+  </si>
+  <si>
+    <t>Targetable</t>
   </si>
 </sst>
 </file>
@@ -1701,18 +1647,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1736,26 +1682,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1798,10 +1744,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F7"/>
+    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,11 +1757,10 @@
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1832,133 +1777,121 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E7" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"n,y"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7" xr:uid="{00000000-0002-0000-0100-000003000000}">
-      <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2008,7 +1941,7 @@
         <v>undx</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2017,7 +1950,7 @@
         <v>dx</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2026,10 +1959,10 @@
         <v>linked</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2038,10 +1971,10 @@
         <v>tx</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2050,7 +1983,7 @@
         <v>lost</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2059,10 +1992,10 @@
         <v>vs</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -2072,10 +2005,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="165" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,11 +2017,10 @@
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2096,167 +2028,140 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E8" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>"y,n"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -2264,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,11 +2185,10 @@
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2292,39 +2196,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2">
@@ -2333,22 +2234,21 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2">
@@ -2358,25 +2258,22 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -2385,24 +2282,21 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="2">
@@ -2411,22 +2305,21 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="2">
@@ -2436,25 +2329,22 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2">
@@ -2465,24 +2355,21 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D8" s="2">
         <v>0.2</v>
@@ -2493,24 +2380,21 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2">
         <v>0.16</v>
@@ -2523,16 +2407,13 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2541,9 +2422,8 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2552,9 +2432,8 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2563,9 +2442,8 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -2574,9 +2452,8 @@
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2585,9 +2462,8 @@
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -2596,9 +2472,8 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2607,32 +2482,28 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18 C2:C19" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>",number,probability,duration,proportion"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:I19" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H19" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"y,n"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2658,42 +2529,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2701,10 +2572,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -2712,10 +2583,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>

</xml_diff>

<commit_message>
Modify framework to prevent divide by zeros
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_hiv.xlsx
+++ b/tests/frameworks/framework_hiv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BAA615-B9F4-48D3-974E-999C155647A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2ECFD44-012B-4AC2-B9FC-3734781F413F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="28560" windowHeight="14175" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -1087,9 +1087,6 @@
     <t>num_diag</t>
   </si>
   <si>
-    <t>num_diag/undx</t>
-  </si>
-  <si>
     <t>num_initiate</t>
   </si>
   <si>
@@ -1183,9 +1180,6 @@
     <t>duration</t>
   </si>
   <si>
-    <t>num_initiate/linked</t>
-  </si>
-  <si>
     <t>Time after initiating ART to achieve viral suppression (years)</t>
   </si>
   <si>
@@ -1208,6 +1202,12 @@
   </si>
   <si>
     <t>Targetable</t>
+  </si>
+  <si>
+    <t>num_diag/max(undx,num_diag)</t>
+  </si>
+  <si>
+    <t>num_initiate/max(linked,num_initiate)</t>
   </si>
 </sst>
 </file>
@@ -1647,18 +1647,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1690,18 +1690,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1746,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView zoomScale="166" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1854,10 +1854,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -1872,10 +1872,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
@@ -1950,7 +1950,7 @@
         <v>dx</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
         <v>21</v>
       </c>
       <c r="G5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1983,7 +1983,7 @@
         <v>lost</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>vs</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -2042,16 +2042,16 @@
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2059,50 +2059,50 @@
         <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2113,30 +2113,30 @@
         <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2171,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2183,7 +2183,7 @@
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
     <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2211,7 +2211,7 @@
         <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>32</v>
@@ -2222,7 +2222,7 @@
         <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>33</v>
@@ -2237,7 +2237,7 @@
         <v>6</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2258,7 +2258,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>7</v>
@@ -2267,13 +2267,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -2285,15 +2285,15 @@
         <v>7</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>33</v>
@@ -2308,7 +2308,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2316,7 +2316,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>27</v>
@@ -2329,7 +2329,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>7</v>
@@ -2358,18 +2358,18 @@
         <v>7</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="2">
         <v>0.2</v>
@@ -2383,15 +2383,15 @@
         <v>6</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>27</v>
@@ -2410,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>23</v>
@@ -2553,18 +2553,18 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -2583,10 +2583,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>

</xml_diff>